<commit_message>
Added calendar and senior citizen insert
</commit_message>
<xml_diff>
--- a/test/FORM Fields.xlsx
+++ b/test/FORM Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cswd\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8FC84F-BC61-46C5-AF28-4D7A729D7E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365FAB7-C791-4A61-9A5C-73930730BFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A17AED3D-BB50-41F5-93ED-92BC410CDAD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="163">
   <si>
     <t>{</t>
   </si>
@@ -414,6 +414,117 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "ASUNCION"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "SABANDAL"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "Female"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "Widowed"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "srCitizenDOB",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "1942-01-12"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "AKLAN"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "email",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "asuncionmontealegre@gmail.com"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "09091072865"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "religion",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "CATHOLIC"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "hasPension",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "Meron"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "whatPension",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "SSS"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "howMuchPension",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "6000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "spouseLastName",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "spouseFirstName",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "VERGILIO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "spouseMiddleName",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "SOBERANO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "spouseSuffix",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": ""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "spouseDOB",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "1942-08-07"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "numberOfChildren",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "totalHousemate",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "MILA ROSA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "srCitizenChildDOB",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "1965-07-20"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "childTelephone",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "childBarangay",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "childAddress",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "value": "BLOCK 7 LOT 2 ROSE POINTE SUBD BRGY. TAGAPO SANTA ROSA LAGUNA"</t>
   </si>
 </sst>
 </file>
@@ -765,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409FE08B-E30D-44BC-BE3F-CFC0D785988F}">
-  <dimension ref="A2:C210"/>
+  <dimension ref="A2:C330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213:B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2178,596 @@
         <v>125</v>
       </c>
     </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B266" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B271" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B289" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B290" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B291" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B292" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B293" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B294" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B295" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B296" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B297" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B298" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B299" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B300" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B301" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B302" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B303" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B304" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B305" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B306" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B307" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B308" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B309" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B310" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B311" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B312" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B313" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B314" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B315" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B321" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B324" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>